<commit_message>
MTTC and FTF changes
</commit_message>
<xml_diff>
--- a/svmx/test_lab/test_cases/analytics/an_excleData/FTF_data.xlsx
+++ b/svmx/test_lab/test_cases/analytics/an_excleData/FTF_data.xlsx
@@ -53,9 +53,6 @@
     <t>Site</t>
   </si>
   <si>
-    <t>a0Nq0000003PBZS</t>
-  </si>
-  <si>
     <t>System.Today()</t>
   </si>
   <si>
@@ -147,6 +144,9 @@
   </si>
   <si>
     <t>Case case_3= new Case (Status = 'Closed',Origin='Phone' );insert case_3 ;</t>
+  </si>
+  <si>
+    <t>a0Nq0000003PKUcEAO</t>
   </si>
 </sst>
 </file>
@@ -598,7 +598,7 @@
   <dimension ref="A1:Q6"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -635,16 +635,16 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="H1" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>4</v>
@@ -653,60 +653,60 @@
         <v>7</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="M1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="O1" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="P1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="112" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>37</v>
-      </c>
       <c r="D2" s="2" t="s">
-        <v>8</v>
+        <v>39</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>6</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L2" s="5">
         <v>43020.416666666664</v>
@@ -715,10 +715,10 @@
         <v>43020.458333333336</v>
       </c>
       <c r="N2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="O2" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="P2" s="1">
         <v>30</v>
@@ -729,54 +729,54 @@
     </row>
     <row r="3" spans="1:17" ht="64" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L4" s="6"/>
     </row>
     <row r="5" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>37</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L5" s="6">
         <v>43020.416666666664</v>
@@ -787,7 +787,7 @@
     </row>
     <row r="6" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="I6" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M6" s="7"/>
     </row>

</xml_diff>